<commit_message>
Final value fee â€“ fixed
</commit_message>
<xml_diff>
--- a/Raw Sales Data/Vandey.xlsx
+++ b/Raw Sales Data/Vandey.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\email\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PURU AARU\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2CC6C-1292-42D7-BA3C-D37E209DA836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3966,9 +3967,6 @@
     <t xml:space="preserve">Estimated release on 2 Sep. </t>
   </si>
   <si>
-    <t>Final value fee – fixed</t>
-  </si>
-  <si>
     <t>Final value fee – variable</t>
   </si>
   <si>
@@ -4936,12 +4934,15 @@
   </si>
   <si>
     <t>19/12/2024 23:59:59 PM GMT</t>
+  </si>
+  <si>
+    <t>Final value fee â€“ fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5743,11 +5744,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL544"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5834,7 +5835,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -5842,7 +5843,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -5850,7 +5851,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -5936,10 +5937,10 @@
         <v>37</v>
       </c>
       <c r="AB12" t="s">
+        <v>1638</v>
+      </c>
+      <c r="AC12" t="s">
         <v>1315</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>1316</v>
       </c>
       <c r="AD12" t="s">
         <v>38</v>
@@ -5977,16 +5978,16 @@
         <v>47</v>
       </c>
       <c r="C13" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E13" t="s">
         <v>1317</v>
       </c>
-      <c r="D13" t="s">
-        <v>1317</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>1318</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1319</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -6079,7 +6080,7 @@
         <v>0</v>
       </c>
       <c r="AK13" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="AL13" t="s">
         <v>53</v>
@@ -6093,25 +6094,25 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E14" t="s">
         <v>1317</v>
       </c>
-      <c r="D14" t="s">
-        <v>1317</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>1318</v>
       </c>
-      <c r="F14" t="s">
-        <v>1319</v>
-      </c>
       <c r="G14" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H14" t="s">
         <v>117</v>
       </c>
       <c r="I14" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="J14" t="s">
         <v>58</v>
@@ -6209,16 +6210,16 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E15" t="s">
         <v>1323</v>
       </c>
-      <c r="D15" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>1324</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1325</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
@@ -6311,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="AK15" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="AL15" t="s">
         <v>53</v>
@@ -6325,25 +6326,25 @@
         <v>54</v>
       </c>
       <c r="C16" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E16" t="s">
         <v>1323</v>
       </c>
-      <c r="D16" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>1324</v>
       </c>
-      <c r="F16" t="s">
-        <v>1325</v>
-      </c>
       <c r="G16" t="s">
+        <v>1326</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>1327</v>
-      </c>
-      <c r="H16" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1328</v>
       </c>
       <c r="J16" t="s">
         <v>58</v>
@@ -6441,16 +6442,16 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E17" t="s">
         <v>1329</v>
       </c>
-      <c r="D17" t="s">
-        <v>1329</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>1330</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1331</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
@@ -6543,7 +6544,7 @@
         <v>0</v>
       </c>
       <c r="AK17" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="AL17" t="s">
         <v>53</v>
@@ -6557,16 +6558,16 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E18" t="s">
         <v>1329</v>
       </c>
-      <c r="D18" t="s">
-        <v>1329</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>1330</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1331</v>
       </c>
       <c r="G18" t="s">
         <v>1279</v>
@@ -6575,7 +6576,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="J18" t="s">
         <v>58</v>
@@ -6673,16 +6674,16 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E19" t="s">
         <v>1334</v>
       </c>
-      <c r="D19" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>1335</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1336</v>
       </c>
       <c r="G19" t="s">
         <v>0</v>
@@ -6775,7 +6776,7 @@
         <v>0</v>
       </c>
       <c r="AK19" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="AL19" t="s">
         <v>53</v>
@@ -6789,25 +6790,25 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E20" t="s">
         <v>1334</v>
       </c>
-      <c r="D20" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>1335</v>
       </c>
-      <c r="F20" t="s">
-        <v>1336</v>
-      </c>
       <c r="G20" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="H20" t="s">
         <v>794</v>
       </c>
       <c r="I20" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="J20" t="s">
         <v>58</v>
@@ -6905,16 +6906,16 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E21" t="s">
         <v>1340</v>
       </c>
-      <c r="D21" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>1341</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1342</v>
       </c>
       <c r="G21" t="s">
         <v>0</v>
@@ -7007,7 +7008,7 @@
         <v>0</v>
       </c>
       <c r="AK21" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="AL21" t="s">
         <v>53</v>
@@ -7021,25 +7022,25 @@
         <v>54</v>
       </c>
       <c r="C22" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E22" t="s">
         <v>1340</v>
       </c>
-      <c r="D22" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>1341</v>
       </c>
-      <c r="F22" t="s">
-        <v>1342</v>
-      </c>
       <c r="G22" t="s">
+        <v>1343</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
         <v>1344</v>
-      </c>
-      <c r="H22" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>1345</v>
       </c>
       <c r="J22" t="s">
         <v>58</v>
@@ -7137,16 +7138,16 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E23" t="s">
         <v>1346</v>
       </c>
-      <c r="D23" t="s">
-        <v>1346</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>1347</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1348</v>
       </c>
       <c r="G23" t="s">
         <v>0</v>
@@ -7239,7 +7240,7 @@
         <v>0</v>
       </c>
       <c r="AK23" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AL23" t="s">
         <v>53</v>
@@ -7253,25 +7254,25 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E24" t="s">
         <v>1346</v>
       </c>
-      <c r="D24" t="s">
-        <v>1346</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>1347</v>
       </c>
-      <c r="F24" t="s">
-        <v>1348</v>
-      </c>
       <c r="G24" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="H24" t="s">
         <v>659</v>
       </c>
       <c r="I24" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="J24" t="s">
         <v>58</v>
@@ -7369,16 +7370,16 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E25" t="s">
         <v>1352</v>
       </c>
-      <c r="D25" t="s">
-        <v>1352</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>1353</v>
-      </c>
-      <c r="F25" t="s">
-        <v>1354</v>
       </c>
       <c r="G25" t="s">
         <v>0</v>
@@ -7471,7 +7472,7 @@
         <v>0</v>
       </c>
       <c r="AK25" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="AL25" t="s">
         <v>53</v>
@@ -7485,25 +7486,25 @@
         <v>54</v>
       </c>
       <c r="C26" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E26" t="s">
         <v>1352</v>
       </c>
-      <c r="D26" t="s">
-        <v>1352</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>1353</v>
       </c>
-      <c r="F26" t="s">
-        <v>1354</v>
-      </c>
       <c r="G26" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
         <v>1356</v>
-      </c>
-      <c r="H26" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>1357</v>
       </c>
       <c r="J26" t="s">
         <v>58</v>
@@ -7601,16 +7602,16 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E27" t="s">
         <v>1358</v>
       </c>
-      <c r="D27" t="s">
-        <v>1358</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>1359</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1360</v>
       </c>
       <c r="G27" t="s">
         <v>0</v>
@@ -7703,7 +7704,7 @@
         <v>0</v>
       </c>
       <c r="AK27" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="AL27" t="s">
         <v>53</v>
@@ -7717,25 +7718,25 @@
         <v>54</v>
       </c>
       <c r="C28" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E28" t="s">
         <v>1358</v>
       </c>
-      <c r="D28" t="s">
-        <v>1358</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>1359</v>
       </c>
-      <c r="F28" t="s">
-        <v>1360</v>
-      </c>
       <c r="G28" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="H28" t="s">
         <v>478</v>
       </c>
       <c r="I28" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="J28" t="s">
         <v>58</v>
@@ -7833,16 +7834,16 @@
         <v>47</v>
       </c>
       <c r="C29" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E29" t="s">
         <v>1364</v>
       </c>
-      <c r="D29" t="s">
-        <v>1364</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>1365</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1366</v>
       </c>
       <c r="G29" t="s">
         <v>0</v>
@@ -7935,7 +7936,7 @@
         <v>0</v>
       </c>
       <c r="AK29" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="AL29" t="s">
         <v>53</v>
@@ -7949,25 +7950,25 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E30" t="s">
         <v>1364</v>
       </c>
-      <c r="D30" t="s">
-        <v>1364</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>1365</v>
       </c>
-      <c r="F30" t="s">
-        <v>1366</v>
-      </c>
       <c r="G30" t="s">
+        <v>1367</v>
+      </c>
+      <c r="H30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
         <v>1368</v>
-      </c>
-      <c r="H30" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>1369</v>
       </c>
       <c r="J30" t="s">
         <v>58</v>
@@ -8065,16 +8066,16 @@
         <v>47</v>
       </c>
       <c r="C31" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E31" t="s">
         <v>1370</v>
       </c>
-      <c r="D31" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>1371</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1372</v>
       </c>
       <c r="G31" t="s">
         <v>0</v>
@@ -8167,7 +8168,7 @@
         <v>0</v>
       </c>
       <c r="AK31" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="AL31" t="s">
         <v>53</v>
@@ -8181,25 +8182,25 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E32" t="s">
         <v>1370</v>
       </c>
-      <c r="D32" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>1371</v>
       </c>
-      <c r="F32" t="s">
-        <v>1372</v>
-      </c>
       <c r="G32" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="H32" t="s">
         <v>674</v>
       </c>
       <c r="I32" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="J32" t="s">
         <v>58</v>
@@ -8297,16 +8298,16 @@
         <v>47</v>
       </c>
       <c r="C33" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E33" t="s">
         <v>1376</v>
       </c>
-      <c r="D33" t="s">
-        <v>1376</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>1377</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1378</v>
       </c>
       <c r="G33" t="s">
         <v>0</v>
@@ -8399,7 +8400,7 @@
         <v>0</v>
       </c>
       <c r="AK33" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="AL33" t="s">
         <v>53</v>
@@ -8413,25 +8414,25 @@
         <v>54</v>
       </c>
       <c r="C34" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E34" t="s">
         <v>1376</v>
       </c>
-      <c r="D34" t="s">
-        <v>1376</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>1377</v>
       </c>
-      <c r="F34" t="s">
-        <v>1378</v>
-      </c>
       <c r="G34" t="s">
+        <v>1379</v>
+      </c>
+      <c r="H34" t="s">
         <v>1380</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>1381</v>
-      </c>
-      <c r="I34" t="s">
-        <v>1382</v>
       </c>
       <c r="J34" t="s">
         <v>58</v>
@@ -8529,16 +8530,16 @@
         <v>47</v>
       </c>
       <c r="C35" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E35" t="s">
         <v>1383</v>
       </c>
-      <c r="D35" t="s">
-        <v>1383</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>1384</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1385</v>
       </c>
       <c r="G35" t="s">
         <v>0</v>
@@ -8631,7 +8632,7 @@
         <v>0</v>
       </c>
       <c r="AK35" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="AL35" t="s">
         <v>53</v>
@@ -8645,16 +8646,16 @@
         <v>47</v>
       </c>
       <c r="C36" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E36" t="s">
         <v>1387</v>
       </c>
-      <c r="D36" t="s">
-        <v>1387</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>1388</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1389</v>
       </c>
       <c r="G36" t="s">
         <v>0</v>
@@ -8747,7 +8748,7 @@
         <v>0</v>
       </c>
       <c r="AK36" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="AL36" t="s">
         <v>53</v>
@@ -8761,25 +8762,25 @@
         <v>54</v>
       </c>
       <c r="C37" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E37" t="s">
         <v>1383</v>
       </c>
-      <c r="D37" t="s">
-        <v>1383</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>1384</v>
       </c>
-      <c r="F37" t="s">
-        <v>1385</v>
-      </c>
       <c r="G37" t="s">
+        <v>1390</v>
+      </c>
+      <c r="H37" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
         <v>1391</v>
-      </c>
-      <c r="H37" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>1392</v>
       </c>
       <c r="J37" t="s">
         <v>58</v>
@@ -8877,16 +8878,16 @@
         <v>54</v>
       </c>
       <c r="C38" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E38" t="s">
         <v>1387</v>
       </c>
-      <c r="D38" t="s">
-        <v>1387</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>1388</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1389</v>
       </c>
       <c r="G38" t="s">
         <v>303</v>
@@ -8895,7 +8896,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="J38" t="s">
         <v>58</v>
@@ -8993,16 +8994,16 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E39" t="s">
         <v>1394</v>
       </c>
-      <c r="D39" t="s">
-        <v>1394</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>1395</v>
-      </c>
-      <c r="F39" t="s">
-        <v>1396</v>
       </c>
       <c r="G39" t="s">
         <v>0</v>
@@ -9095,7 +9096,7 @@
         <v>0</v>
       </c>
       <c r="AK39" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="AL39" t="s">
         <v>53</v>
@@ -9109,16 +9110,16 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E40" t="s">
         <v>1398</v>
       </c>
-      <c r="D40" t="s">
-        <v>1398</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>1399</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1400</v>
       </c>
       <c r="G40" t="s">
         <v>0</v>
@@ -9211,7 +9212,7 @@
         <v>0</v>
       </c>
       <c r="AK40" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="AL40" t="s">
         <v>53</v>
@@ -9225,25 +9226,25 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E41" t="s">
         <v>1394</v>
       </c>
-      <c r="D41" t="s">
-        <v>1394</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>1395</v>
       </c>
-      <c r="F41" t="s">
-        <v>1396</v>
-      </c>
       <c r="G41" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H41" t="s">
         <v>93</v>
       </c>
       <c r="I41" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="J41" t="s">
         <v>58</v>
@@ -9341,25 +9342,25 @@
         <v>54</v>
       </c>
       <c r="C42" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E42" t="s">
         <v>1398</v>
       </c>
-      <c r="D42" t="s">
-        <v>1398</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>1399</v>
       </c>
-      <c r="F42" t="s">
-        <v>1400</v>
-      </c>
       <c r="G42" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H42" t="s">
         <v>1045</v>
       </c>
       <c r="I42" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="J42" t="s">
         <v>58</v>
@@ -9457,16 +9458,16 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E43" t="s">
         <v>1406</v>
       </c>
-      <c r="D43" t="s">
-        <v>1406</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>1407</v>
-      </c>
-      <c r="F43" t="s">
-        <v>1408</v>
       </c>
       <c r="G43" t="s">
         <v>0</v>
@@ -9559,7 +9560,7 @@
         <v>0</v>
       </c>
       <c r="AK43" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="AL43" t="s">
         <v>53</v>
@@ -9573,25 +9574,25 @@
         <v>54</v>
       </c>
       <c r="C44" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E44" t="s">
         <v>1406</v>
       </c>
-      <c r="D44" t="s">
-        <v>1406</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>1407</v>
       </c>
-      <c r="F44" t="s">
-        <v>1408</v>
-      </c>
       <c r="G44" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="H44" t="s">
         <v>347</v>
       </c>
       <c r="I44" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="J44" t="s">
         <v>58</v>
@@ -9689,16 +9690,16 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E45" t="s">
         <v>1412</v>
       </c>
-      <c r="D45" t="s">
-        <v>1412</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>1413</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1414</v>
       </c>
       <c r="G45" t="s">
         <v>0</v>
@@ -9791,7 +9792,7 @@
         <v>0</v>
       </c>
       <c r="AK45" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="AL45" t="s">
         <v>53</v>
@@ -9805,16 +9806,16 @@
         <v>54</v>
       </c>
       <c r="C46" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E46" t="s">
         <v>1412</v>
       </c>
-      <c r="D46" t="s">
-        <v>1412</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>1413</v>
-      </c>
-      <c r="F46" t="s">
-        <v>1414</v>
       </c>
       <c r="G46" t="s">
         <v>1285</v>
@@ -9823,7 +9824,7 @@
         <v>1002</v>
       </c>
       <c r="I46" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="J46" t="s">
         <v>58</v>
@@ -9921,16 +9922,16 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E47" t="s">
         <v>1417</v>
       </c>
-      <c r="D47" t="s">
-        <v>1417</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>1418</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1419</v>
       </c>
       <c r="G47" t="s">
         <v>0</v>
@@ -10023,7 +10024,7 @@
         <v>0</v>
       </c>
       <c r="AK47" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="AL47" t="s">
         <v>53</v>
@@ -10037,25 +10038,25 @@
         <v>54</v>
       </c>
       <c r="C48" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E48" t="s">
         <v>1417</v>
       </c>
-      <c r="D48" t="s">
-        <v>1417</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>1418</v>
       </c>
-      <c r="F48" t="s">
-        <v>1419</v>
-      </c>
       <c r="G48" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="H48" t="s">
         <v>846</v>
       </c>
       <c r="I48" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="J48" t="s">
         <v>58</v>
@@ -10153,16 +10154,16 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E49" t="s">
         <v>1423</v>
       </c>
-      <c r="D49" t="s">
-        <v>1423</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>1424</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1425</v>
       </c>
       <c r="G49" t="s">
         <v>0</v>
@@ -10255,7 +10256,7 @@
         <v>0</v>
       </c>
       <c r="AK49" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="AL49" t="s">
         <v>53</v>
@@ -10269,25 +10270,25 @@
         <v>54</v>
       </c>
       <c r="C50" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E50" t="s">
         <v>1423</v>
       </c>
-      <c r="D50" t="s">
-        <v>1423</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>1424</v>
       </c>
-      <c r="F50" t="s">
-        <v>1425</v>
-      </c>
       <c r="G50" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="H50" t="s">
         <v>93</v>
       </c>
       <c r="I50" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="J50" t="s">
         <v>58</v>
@@ -10385,16 +10386,16 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E51" t="s">
         <v>1429</v>
       </c>
-      <c r="D51" t="s">
-        <v>1429</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>1430</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1431</v>
       </c>
       <c r="G51" t="s">
         <v>0</v>
@@ -10487,7 +10488,7 @@
         <v>0</v>
       </c>
       <c r="AK51" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="AL51" t="s">
         <v>53</v>
@@ -10501,25 +10502,25 @@
         <v>54</v>
       </c>
       <c r="C52" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E52" t="s">
         <v>1429</v>
       </c>
-      <c r="D52" t="s">
-        <v>1429</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>1430</v>
       </c>
-      <c r="F52" t="s">
-        <v>1431</v>
-      </c>
       <c r="G52" t="s">
+        <v>1432</v>
+      </c>
+      <c r="H52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
         <v>1433</v>
-      </c>
-      <c r="H52" t="s">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>1434</v>
       </c>
       <c r="J52" t="s">
         <v>58</v>
@@ -10617,16 +10618,16 @@
         <v>47</v>
       </c>
       <c r="C53" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E53" t="s">
         <v>1435</v>
       </c>
-      <c r="D53" t="s">
-        <v>1435</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>1436</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1437</v>
       </c>
       <c r="G53" t="s">
         <v>0</v>
@@ -10719,7 +10720,7 @@
         <v>0</v>
       </c>
       <c r="AK53" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="AL53" t="s">
         <v>53</v>
@@ -10733,16 +10734,16 @@
         <v>54</v>
       </c>
       <c r="C54" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E54" t="s">
         <v>1435</v>
       </c>
-      <c r="D54" t="s">
-        <v>1435</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>1436</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1437</v>
       </c>
       <c r="G54" t="s">
         <v>603</v>
@@ -10751,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="J54" t="s">
         <v>58</v>
@@ -10849,16 +10850,16 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E55" t="s">
         <v>1440</v>
       </c>
-      <c r="D55" t="s">
-        <v>1440</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>1441</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1442</v>
       </c>
       <c r="G55" t="s">
         <v>0</v>
@@ -10951,7 +10952,7 @@
         <v>0</v>
       </c>
       <c r="AK55" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="AL55" t="s">
         <v>53</v>
@@ -10965,25 +10966,25 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E56" t="s">
         <v>1440</v>
       </c>
-      <c r="D56" t="s">
-        <v>1440</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>1441</v>
       </c>
-      <c r="F56" t="s">
-        <v>1442</v>
-      </c>
       <c r="G56" t="s">
+        <v>1443</v>
+      </c>
+      <c r="H56" t="s">
         <v>1444</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>1445</v>
-      </c>
-      <c r="I56" t="s">
-        <v>1446</v>
       </c>
       <c r="J56" t="s">
         <v>58</v>
@@ -11081,16 +11082,16 @@
         <v>47</v>
       </c>
       <c r="C57" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E57" t="s">
         <v>1447</v>
       </c>
-      <c r="D57" t="s">
-        <v>1447</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>1448</v>
-      </c>
-      <c r="F57" t="s">
-        <v>1449</v>
       </c>
       <c r="G57" t="s">
         <v>0</v>
@@ -11183,7 +11184,7 @@
         <v>0</v>
       </c>
       <c r="AK57" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="AL57" t="s">
         <v>53</v>
@@ -11197,25 +11198,25 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E58" t="s">
         <v>1447</v>
       </c>
-      <c r="D58" t="s">
-        <v>1447</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>1448</v>
       </c>
-      <c r="F58" t="s">
-        <v>1449</v>
-      </c>
       <c r="G58" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="H58" t="s">
         <v>1235</v>
       </c>
       <c r="I58" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="J58" t="s">
         <v>58</v>
@@ -11313,16 +11314,16 @@
         <v>47</v>
       </c>
       <c r="C59" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E59" t="s">
         <v>1453</v>
       </c>
-      <c r="D59" t="s">
-        <v>1453</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>1454</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1455</v>
       </c>
       <c r="G59" t="s">
         <v>0</v>
@@ -11415,7 +11416,7 @@
         <v>0</v>
       </c>
       <c r="AK59" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="AL59" t="s">
         <v>53</v>
@@ -11429,25 +11430,25 @@
         <v>54</v>
       </c>
       <c r="C60" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E60" t="s">
         <v>1453</v>
       </c>
-      <c r="D60" t="s">
-        <v>1453</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>1454</v>
       </c>
-      <c r="F60" t="s">
-        <v>1455</v>
-      </c>
       <c r="G60" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H60" t="s">
         <v>1045</v>
       </c>
       <c r="I60" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="J60" t="s">
         <v>58</v>
@@ -11545,16 +11546,16 @@
         <v>47</v>
       </c>
       <c r="C61" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E61" t="s">
         <v>1459</v>
       </c>
-      <c r="D61" t="s">
-        <v>1459</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>1460</v>
-      </c>
-      <c r="F61" t="s">
-        <v>1461</v>
       </c>
       <c r="G61" t="s">
         <v>0</v>
@@ -11647,7 +11648,7 @@
         <v>0</v>
       </c>
       <c r="AK61" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="AL61" t="s">
         <v>53</v>
@@ -11661,16 +11662,16 @@
         <v>54</v>
       </c>
       <c r="C62" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E62" t="s">
         <v>1459</v>
       </c>
-      <c r="D62" t="s">
-        <v>1459</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>1460</v>
-      </c>
-      <c r="F62" t="s">
-        <v>1461</v>
       </c>
       <c r="G62" t="s">
         <v>156</v>
@@ -11679,7 +11680,7 @@
         <v>93</v>
       </c>
       <c r="I62" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="J62" t="s">
         <v>58</v>
@@ -11777,16 +11778,16 @@
         <v>47</v>
       </c>
       <c r="C63" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E63" t="s">
         <v>1464</v>
       </c>
-      <c r="D63" t="s">
-        <v>1464</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>1465</v>
-      </c>
-      <c r="F63" t="s">
-        <v>1466</v>
       </c>
       <c r="G63" t="s">
         <v>0</v>
@@ -11879,7 +11880,7 @@
         <v>0</v>
       </c>
       <c r="AK63" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="AL63" t="s">
         <v>53</v>
@@ -11893,25 +11894,25 @@
         <v>54</v>
       </c>
       <c r="C64" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E64" t="s">
         <v>1464</v>
       </c>
-      <c r="D64" t="s">
-        <v>1464</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>1465</v>
       </c>
-      <c r="F64" t="s">
-        <v>1466</v>
-      </c>
       <c r="G64" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
         <v>1468</v>
-      </c>
-      <c r="H64" t="s">
-        <v>0</v>
-      </c>
-      <c r="I64" t="s">
-        <v>1469</v>
       </c>
       <c r="J64" t="s">
         <v>58</v>
@@ -12009,16 +12010,16 @@
         <v>47</v>
       </c>
       <c r="C65" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E65" t="s">
         <v>1470</v>
       </c>
-      <c r="D65" t="s">
-        <v>1470</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>1471</v>
-      </c>
-      <c r="F65" t="s">
-        <v>1472</v>
       </c>
       <c r="G65" t="s">
         <v>0</v>
@@ -12111,7 +12112,7 @@
         <v>0</v>
       </c>
       <c r="AK65" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="AL65" t="s">
         <v>53</v>
@@ -12125,16 +12126,16 @@
         <v>54</v>
       </c>
       <c r="C66" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E66" t="s">
         <v>1470</v>
       </c>
-      <c r="D66" t="s">
-        <v>1470</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>1471</v>
-      </c>
-      <c r="F66" t="s">
-        <v>1472</v>
       </c>
       <c r="G66" t="s">
         <v>234</v>
@@ -12143,7 +12144,7 @@
         <v>234</v>
       </c>
       <c r="I66" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="J66" t="s">
         <v>58</v>
@@ -12241,16 +12242,16 @@
         <v>47</v>
       </c>
       <c r="C67" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1474</v>
+      </c>
+      <c r="E67" t="s">
         <v>1475</v>
       </c>
-      <c r="D67" t="s">
-        <v>1475</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>1476</v>
-      </c>
-      <c r="F67" t="s">
-        <v>1477</v>
       </c>
       <c r="G67" t="s">
         <v>0</v>
@@ -12343,7 +12344,7 @@
         <v>0</v>
       </c>
       <c r="AK67" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="AL67" t="s">
         <v>53</v>
@@ -12357,16 +12358,16 @@
         <v>47</v>
       </c>
       <c r="C68" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E68" t="s">
         <v>1479</v>
       </c>
-      <c r="D68" t="s">
-        <v>1479</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>1480</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1481</v>
       </c>
       <c r="G68" t="s">
         <v>0</v>
@@ -12459,7 +12460,7 @@
         <v>0</v>
       </c>
       <c r="AK68" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="AL68" t="s">
         <v>53</v>
@@ -12473,25 +12474,25 @@
         <v>54</v>
       </c>
       <c r="C69" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E69" t="s">
         <v>1479</v>
       </c>
-      <c r="D69" t="s">
-        <v>1479</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>1480</v>
       </c>
-      <c r="F69" t="s">
-        <v>1481</v>
-      </c>
       <c r="G69" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="H69" t="s">
         <v>241</v>
       </c>
       <c r="I69" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="J69" t="s">
         <v>58</v>
@@ -12589,25 +12590,25 @@
         <v>54</v>
       </c>
       <c r="C70" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1474</v>
+      </c>
+      <c r="E70" t="s">
         <v>1475</v>
       </c>
-      <c r="D70" t="s">
-        <v>1475</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>1476</v>
       </c>
-      <c r="F70" t="s">
-        <v>1477</v>
-      </c>
       <c r="G70" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="H70" t="s">
         <v>1235</v>
       </c>
       <c r="I70" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="J70" t="s">
         <v>58</v>
@@ -12705,16 +12706,16 @@
         <v>47</v>
       </c>
       <c r="C71" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E71" t="s">
         <v>1487</v>
       </c>
-      <c r="D71" t="s">
-        <v>1487</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>1488</v>
-      </c>
-      <c r="F71" t="s">
-        <v>1489</v>
       </c>
       <c r="G71" t="s">
         <v>0</v>
@@ -12807,7 +12808,7 @@
         <v>0</v>
       </c>
       <c r="AK71" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="AL71" t="s">
         <v>53</v>
@@ -12821,16 +12822,16 @@
         <v>54</v>
       </c>
       <c r="C72" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E72" t="s">
         <v>1487</v>
       </c>
-      <c r="D72" t="s">
-        <v>1487</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>1488</v>
-      </c>
-      <c r="F72" t="s">
-        <v>1489</v>
       </c>
       <c r="G72" t="s">
         <v>156</v>
@@ -12839,7 +12840,7 @@
         <v>93</v>
       </c>
       <c r="I72" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="J72" t="s">
         <v>58</v>
@@ -12937,16 +12938,16 @@
         <v>47</v>
       </c>
       <c r="C73" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E73" t="s">
         <v>1492</v>
       </c>
-      <c r="D73" t="s">
-        <v>1492</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>1493</v>
-      </c>
-      <c r="F73" t="s">
-        <v>1494</v>
       </c>
       <c r="G73" t="s">
         <v>0</v>
@@ -13039,7 +13040,7 @@
         <v>0</v>
       </c>
       <c r="AK73" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="AL73" t="s">
         <v>53</v>
@@ -13053,25 +13054,25 @@
         <v>54</v>
       </c>
       <c r="C74" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1491</v>
+      </c>
+      <c r="E74" t="s">
         <v>1492</v>
       </c>
-      <c r="D74" t="s">
-        <v>1492</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>1493</v>
       </c>
-      <c r="F74" t="s">
-        <v>1494</v>
-      </c>
       <c r="G74" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="H74" t="s">
         <v>551</v>
       </c>
       <c r="I74" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="J74" t="s">
         <v>58</v>
@@ -13169,16 +13170,16 @@
         <v>47</v>
       </c>
       <c r="C75" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1497</v>
+      </c>
+      <c r="E75" t="s">
         <v>1498</v>
       </c>
-      <c r="D75" t="s">
-        <v>1498</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>1499</v>
-      </c>
-      <c r="F75" t="s">
-        <v>1500</v>
       </c>
       <c r="G75" t="s">
         <v>0</v>
@@ -13271,7 +13272,7 @@
         <v>0</v>
       </c>
       <c r="AK75" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="AL75" t="s">
         <v>53</v>
@@ -13285,25 +13286,25 @@
         <v>54</v>
       </c>
       <c r="C76" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1497</v>
+      </c>
+      <c r="E76" t="s">
         <v>1498</v>
       </c>
-      <c r="D76" t="s">
-        <v>1498</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>1499</v>
       </c>
-      <c r="F76" t="s">
-        <v>1500</v>
-      </c>
       <c r="G76" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H76" t="s">
         <v>903</v>
       </c>
       <c r="I76" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="J76" t="s">
         <v>58</v>
@@ -13401,16 +13402,16 @@
         <v>47</v>
       </c>
       <c r="C77" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E77" t="s">
         <v>1504</v>
       </c>
-      <c r="D77" t="s">
-        <v>1504</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>1505</v>
-      </c>
-      <c r="F77" t="s">
-        <v>1506</v>
       </c>
       <c r="G77" t="s">
         <v>0</v>
@@ -13503,7 +13504,7 @@
         <v>0</v>
       </c>
       <c r="AK77" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="AL77" t="s">
         <v>53</v>
@@ -13517,25 +13518,25 @@
         <v>54</v>
       </c>
       <c r="C78" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E78" t="s">
         <v>1504</v>
       </c>
-      <c r="D78" t="s">
-        <v>1504</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>1505</v>
       </c>
-      <c r="F78" t="s">
-        <v>1506</v>
-      </c>
       <c r="G78" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="H78" t="s">
         <v>478</v>
       </c>
       <c r="I78" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="J78" t="s">
         <v>58</v>
@@ -13633,16 +13634,16 @@
         <v>47</v>
       </c>
       <c r="C79" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1508</v>
+      </c>
+      <c r="E79" t="s">
         <v>1509</v>
       </c>
-      <c r="D79" t="s">
-        <v>1509</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>1510</v>
-      </c>
-      <c r="F79" t="s">
-        <v>1511</v>
       </c>
       <c r="G79" t="s">
         <v>0</v>
@@ -13735,7 +13736,7 @@
         <v>0</v>
       </c>
       <c r="AK79" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="AL79" t="s">
         <v>53</v>
@@ -13749,16 +13750,16 @@
         <v>54</v>
       </c>
       <c r="C80" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1508</v>
+      </c>
+      <c r="E80" t="s">
         <v>1509</v>
       </c>
-      <c r="D80" t="s">
-        <v>1509</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>1510</v>
-      </c>
-      <c r="F80" t="s">
-        <v>1511</v>
       </c>
       <c r="G80" t="s">
         <v>608</v>
@@ -13767,7 +13768,7 @@
         <v>609</v>
       </c>
       <c r="I80" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="J80" t="s">
         <v>58</v>
@@ -13865,16 +13866,16 @@
         <v>47</v>
       </c>
       <c r="C81" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E81" t="s">
         <v>1514</v>
       </c>
-      <c r="D81" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>1515</v>
-      </c>
-      <c r="F81" t="s">
-        <v>1516</v>
       </c>
       <c r="G81" t="s">
         <v>0</v>
@@ -13967,7 +13968,7 @@
         <v>0</v>
       </c>
       <c r="AK81" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="AL81" t="s">
         <v>53</v>
@@ -13981,16 +13982,16 @@
         <v>54</v>
       </c>
       <c r="C82" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E82" t="s">
         <v>1514</v>
       </c>
-      <c r="D82" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>1515</v>
-      </c>
-      <c r="F82" t="s">
-        <v>1516</v>
       </c>
       <c r="G82" t="s">
         <v>156</v>
@@ -13999,7 +14000,7 @@
         <v>93</v>
       </c>
       <c r="I82" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="J82" t="s">
         <v>58</v>
@@ -14097,16 +14098,16 @@
         <v>47</v>
       </c>
       <c r="C83" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E83" t="s">
         <v>1519</v>
       </c>
-      <c r="D83" t="s">
-        <v>1519</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>1520</v>
-      </c>
-      <c r="F83" t="s">
-        <v>1521</v>
       </c>
       <c r="G83" t="s">
         <v>0</v>
@@ -14199,7 +14200,7 @@
         <v>0</v>
       </c>
       <c r="AK83" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="AL83" t="s">
         <v>53</v>
@@ -14213,16 +14214,16 @@
         <v>47</v>
       </c>
       <c r="C84" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E84" t="s">
         <v>1523</v>
       </c>
-      <c r="D84" t="s">
-        <v>1523</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>1524</v>
-      </c>
-      <c r="F84" t="s">
-        <v>1525</v>
       </c>
       <c r="G84" t="s">
         <v>0</v>
@@ -14315,7 +14316,7 @@
         <v>0</v>
       </c>
       <c r="AK84" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="AL84" t="s">
         <v>53</v>
@@ -14329,25 +14330,25 @@
         <v>54</v>
       </c>
       <c r="C85" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E85" t="s">
         <v>1519</v>
       </c>
-      <c r="D85" t="s">
-        <v>1519</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>1520</v>
       </c>
-      <c r="F85" t="s">
-        <v>1521</v>
-      </c>
       <c r="G85" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H85" t="s">
         <v>117</v>
       </c>
       <c r="I85" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="J85" t="s">
         <v>58</v>
@@ -14445,16 +14446,16 @@
         <v>47</v>
       </c>
       <c r="C86" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E86" t="s">
         <v>1528</v>
       </c>
-      <c r="D86" t="s">
-        <v>1528</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>1529</v>
-      </c>
-      <c r="F86" t="s">
-        <v>1530</v>
       </c>
       <c r="G86" t="s">
         <v>0</v>
@@ -14547,7 +14548,7 @@
         <v>0</v>
       </c>
       <c r="AK86" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="AL86" t="s">
         <v>53</v>
@@ -14561,16 +14562,16 @@
         <v>54</v>
       </c>
       <c r="C87" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E87" t="s">
         <v>1523</v>
       </c>
-      <c r="D87" t="s">
-        <v>1523</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>1524</v>
-      </c>
-      <c r="F87" t="s">
-        <v>1525</v>
       </c>
       <c r="G87" t="s">
         <v>564</v>
@@ -14579,7 +14580,7 @@
         <v>565</v>
       </c>
       <c r="I87" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="J87" t="s">
         <v>58</v>
@@ -14677,16 +14678,16 @@
         <v>54</v>
       </c>
       <c r="C88" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E88" t="s">
         <v>1528</v>
       </c>
-      <c r="D88" t="s">
-        <v>1528</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>1529</v>
-      </c>
-      <c r="F88" t="s">
-        <v>1530</v>
       </c>
       <c r="G88" t="s">
         <v>650</v>
@@ -14695,7 +14696,7 @@
         <v>651</v>
       </c>
       <c r="I88" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="J88" t="s">
         <v>58</v>
@@ -14793,16 +14794,16 @@
         <v>47</v>
       </c>
       <c r="C89" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E89" t="s">
         <v>1534</v>
       </c>
-      <c r="D89" t="s">
-        <v>1534</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>1535</v>
-      </c>
-      <c r="F89" t="s">
-        <v>1536</v>
       </c>
       <c r="G89" t="s">
         <v>0</v>
@@ -14895,7 +14896,7 @@
         <v>0</v>
       </c>
       <c r="AK89" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="AL89" t="s">
         <v>53</v>
@@ -14909,25 +14910,25 @@
         <v>54</v>
       </c>
       <c r="C90" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E90" t="s">
         <v>1534</v>
       </c>
-      <c r="D90" t="s">
-        <v>1534</v>
-      </c>
-      <c r="E90" t="s">
+      <c r="F90" t="s">
         <v>1535</v>
       </c>
-      <c r="F90" t="s">
-        <v>1536</v>
-      </c>
       <c r="G90" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="H90" t="s">
         <v>339</v>
       </c>
       <c r="I90" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="J90" t="s">
         <v>58</v>
@@ -15025,13 +15026,13 @@
         <v>47</v>
       </c>
       <c r="C91" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E91" t="s">
         <v>1540</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1540</v>
-      </c>
-      <c r="E91" t="s">
-        <v>1541</v>
       </c>
       <c r="F91" t="s">
         <v>218</v>
@@ -15127,7 +15128,7 @@
         <v>0</v>
       </c>
       <c r="AK91" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="AL91" t="s">
         <v>53</v>
@@ -15141,16 +15142,16 @@
         <v>47</v>
       </c>
       <c r="C92" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E92" t="s">
         <v>1543</v>
       </c>
-      <c r="D92" t="s">
-        <v>1543</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>1544</v>
-      </c>
-      <c r="F92" t="s">
-        <v>1545</v>
       </c>
       <c r="G92" t="s">
         <v>0</v>
@@ -15243,7 +15244,7 @@
         <v>0</v>
       </c>
       <c r="AK92" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="AL92" t="s">
         <v>53</v>
@@ -15257,25 +15258,25 @@
         <v>54</v>
       </c>
       <c r="C93" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E93" t="s">
         <v>1540</v>
-      </c>
-      <c r="D93" t="s">
-        <v>1540</v>
-      </c>
-      <c r="E93" t="s">
-        <v>1541</v>
       </c>
       <c r="F93" t="s">
         <v>218</v>
       </c>
       <c r="G93" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="H93" t="s">
         <v>1217</v>
       </c>
       <c r="I93" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="J93" t="s">
         <v>58</v>
@@ -15373,25 +15374,25 @@
         <v>54</v>
       </c>
       <c r="C94" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E94" t="s">
         <v>1543</v>
       </c>
-      <c r="D94" t="s">
-        <v>1543</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>1544</v>
       </c>
-      <c r="F94" t="s">
-        <v>1545</v>
-      </c>
       <c r="G94" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="H94" t="s">
         <v>659</v>
       </c>
       <c r="I94" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="J94" t="s">
         <v>58</v>
@@ -15489,16 +15490,16 @@
         <v>47</v>
       </c>
       <c r="C95" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E95" t="s">
         <v>1551</v>
       </c>
-      <c r="D95" t="s">
-        <v>1551</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>1552</v>
-      </c>
-      <c r="F95" t="s">
-        <v>1553</v>
       </c>
       <c r="G95" t="s">
         <v>0</v>
@@ -15591,7 +15592,7 @@
         <v>0</v>
       </c>
       <c r="AK95" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="AL95" t="s">
         <v>53</v>
@@ -15605,16 +15606,16 @@
         <v>54</v>
       </c>
       <c r="C96" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E96" t="s">
         <v>1551</v>
       </c>
-      <c r="D96" t="s">
-        <v>1551</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>1552</v>
-      </c>
-      <c r="F96" t="s">
-        <v>1553</v>
       </c>
       <c r="G96" t="s">
         <v>515</v>
@@ -15623,7 +15624,7 @@
         <v>117</v>
       </c>
       <c r="I96" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="J96" t="s">
         <v>58</v>
@@ -15721,16 +15722,16 @@
         <v>47</v>
       </c>
       <c r="C97" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E97" t="s">
         <v>1556</v>
       </c>
-      <c r="D97" t="s">
-        <v>1556</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
         <v>1557</v>
-      </c>
-      <c r="F97" t="s">
-        <v>1558</v>
       </c>
       <c r="G97" t="s">
         <v>0</v>
@@ -15823,7 +15824,7 @@
         <v>0</v>
       </c>
       <c r="AK97" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="AL97" t="s">
         <v>53</v>
@@ -15837,25 +15838,25 @@
         <v>54</v>
       </c>
       <c r="C98" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1555</v>
+      </c>
+      <c r="E98" t="s">
         <v>1556</v>
       </c>
-      <c r="D98" t="s">
-        <v>1556</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="F98" t="s">
         <v>1557</v>
       </c>
-      <c r="F98" t="s">
-        <v>1558</v>
-      </c>
       <c r="G98" t="s">
+        <v>1559</v>
+      </c>
+      <c r="H98" t="s">
         <v>1560</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>1561</v>
-      </c>
-      <c r="I98" t="s">
-        <v>1562</v>
       </c>
       <c r="J98" t="s">
         <v>58</v>
@@ -15953,16 +15954,16 @@
         <v>47</v>
       </c>
       <c r="C99" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E99" t="s">
         <v>1563</v>
       </c>
-      <c r="D99" t="s">
-        <v>1563</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>1564</v>
-      </c>
-      <c r="F99" t="s">
-        <v>1565</v>
       </c>
       <c r="G99" t="s">
         <v>0</v>
@@ -16055,7 +16056,7 @@
         <v>0</v>
       </c>
       <c r="AK99" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="AL99" t="s">
         <v>53</v>
@@ -16069,25 +16070,25 @@
         <v>54</v>
       </c>
       <c r="C100" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E100" t="s">
         <v>1563</v>
       </c>
-      <c r="D100" t="s">
-        <v>1563</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>1564</v>
       </c>
-      <c r="F100" t="s">
-        <v>1565</v>
-      </c>
       <c r="G100" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="H100" t="s">
         <v>609</v>
       </c>
       <c r="I100" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="J100" t="s">
         <v>58</v>
@@ -16185,16 +16186,16 @@
         <v>47</v>
       </c>
       <c r="C101" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E101" t="s">
         <v>1569</v>
       </c>
-      <c r="D101" t="s">
-        <v>1569</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>1570</v>
-      </c>
-      <c r="F101" t="s">
-        <v>1571</v>
       </c>
       <c r="G101" t="s">
         <v>0</v>
@@ -16287,7 +16288,7 @@
         <v>0</v>
       </c>
       <c r="AK101" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="AL101" t="s">
         <v>53</v>
@@ -16301,25 +16302,25 @@
         <v>54</v>
       </c>
       <c r="C102" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E102" t="s">
         <v>1569</v>
       </c>
-      <c r="D102" t="s">
-        <v>1569</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>1570</v>
       </c>
-      <c r="F102" t="s">
-        <v>1571</v>
-      </c>
       <c r="G102" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="H102" t="s">
         <v>361</v>
       </c>
       <c r="I102" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="J102" t="s">
         <v>58</v>
@@ -16417,16 +16418,16 @@
         <v>47</v>
       </c>
       <c r="C103" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E103" t="s">
         <v>1575</v>
       </c>
-      <c r="D103" t="s">
-        <v>1575</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>1576</v>
-      </c>
-      <c r="F103" t="s">
-        <v>1577</v>
       </c>
       <c r="G103" t="s">
         <v>0</v>
@@ -16519,7 +16520,7 @@
         <v>0</v>
       </c>
       <c r="AK103" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="AL103" t="s">
         <v>53</v>
@@ -16533,25 +16534,25 @@
         <v>54</v>
       </c>
       <c r="C104" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E104" t="s">
         <v>1575</v>
       </c>
-      <c r="D104" t="s">
-        <v>1575</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>1576</v>
       </c>
-      <c r="F104" t="s">
-        <v>1577</v>
-      </c>
       <c r="G104" t="s">
+        <v>1578</v>
+      </c>
+      <c r="H104" t="s">
         <v>1579</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>1580</v>
-      </c>
-      <c r="I104" t="s">
-        <v>1581</v>
       </c>
       <c r="J104" t="s">
         <v>58</v>
@@ -16649,16 +16650,16 @@
         <v>47</v>
       </c>
       <c r="C105" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E105" t="s">
         <v>1582</v>
       </c>
-      <c r="D105" t="s">
-        <v>1582</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="F105" t="s">
         <v>1583</v>
-      </c>
-      <c r="F105" t="s">
-        <v>1584</v>
       </c>
       <c r="G105" t="s">
         <v>0</v>
@@ -16751,7 +16752,7 @@
         <v>0</v>
       </c>
       <c r="AK105" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="AL105" t="s">
         <v>53</v>
@@ -16765,16 +16766,16 @@
         <v>54</v>
       </c>
       <c r="C106" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E106" t="s">
         <v>1582</v>
       </c>
-      <c r="D106" t="s">
-        <v>1582</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>1583</v>
-      </c>
-      <c r="F106" t="s">
-        <v>1584</v>
       </c>
       <c r="G106" t="s">
         <v>454</v>
@@ -16783,7 +16784,7 @@
         <v>416</v>
       </c>
       <c r="I106" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="J106" t="s">
         <v>58</v>
@@ -16881,16 +16882,16 @@
         <v>47</v>
       </c>
       <c r="C107" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1586</v>
+      </c>
+      <c r="E107" t="s">
         <v>1587</v>
       </c>
-      <c r="D107" t="s">
-        <v>1587</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>1588</v>
-      </c>
-      <c r="F107" t="s">
-        <v>1589</v>
       </c>
       <c r="G107" t="s">
         <v>0</v>
@@ -16983,7 +16984,7 @@
         <v>0</v>
       </c>
       <c r="AK107" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="AL107" t="s">
         <v>53</v>
@@ -16997,25 +16998,25 @@
         <v>54</v>
       </c>
       <c r="C108" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1586</v>
+      </c>
+      <c r="E108" t="s">
         <v>1587</v>
       </c>
-      <c r="D108" t="s">
-        <v>1587</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>1588</v>
       </c>
-      <c r="F108" t="s">
-        <v>1589</v>
-      </c>
       <c r="G108" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="H108" t="s">
         <v>794</v>
       </c>
       <c r="I108" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="J108" t="s">
         <v>58</v>
@@ -17113,16 +17114,16 @@
         <v>47</v>
       </c>
       <c r="C109" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E109" t="s">
         <v>1593</v>
       </c>
-      <c r="D109" t="s">
-        <v>1593</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="F109" t="s">
         <v>1594</v>
-      </c>
-      <c r="F109" t="s">
-        <v>1595</v>
       </c>
       <c r="G109" t="s">
         <v>0</v>
@@ -17215,7 +17216,7 @@
         <v>0</v>
       </c>
       <c r="AK109" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="AL109" t="s">
         <v>53</v>
@@ -17229,25 +17230,25 @@
         <v>54</v>
       </c>
       <c r="C110" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E110" t="s">
         <v>1593</v>
       </c>
-      <c r="D110" t="s">
-        <v>1593</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>1594</v>
       </c>
-      <c r="F110" t="s">
-        <v>1595</v>
-      </c>
       <c r="G110" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="H110" t="s">
         <v>220</v>
       </c>
       <c r="I110" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="J110" t="s">
         <v>58</v>
@@ -17345,16 +17346,16 @@
         <v>47</v>
       </c>
       <c r="C111" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E111" t="s">
         <v>1599</v>
       </c>
-      <c r="D111" t="s">
-        <v>1599</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>1600</v>
-      </c>
-      <c r="F111" t="s">
-        <v>1601</v>
       </c>
       <c r="G111" t="s">
         <v>0</v>
@@ -17447,7 +17448,7 @@
         <v>0</v>
       </c>
       <c r="AK111" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="AL111" t="s">
         <v>53</v>
@@ -17461,25 +17462,25 @@
         <v>54</v>
       </c>
       <c r="C112" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E112" t="s">
         <v>1599</v>
       </c>
-      <c r="D112" t="s">
-        <v>1599</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="F112" t="s">
         <v>1600</v>
       </c>
-      <c r="F112" t="s">
-        <v>1601</v>
-      </c>
       <c r="G112" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H112" t="s">
+        <v>0</v>
+      </c>
+      <c r="I112" t="s">
         <v>1603</v>
-      </c>
-      <c r="H112" t="s">
-        <v>0</v>
-      </c>
-      <c r="I112" t="s">
-        <v>1604</v>
       </c>
       <c r="J112" t="s">
         <v>58</v>
@@ -17577,16 +17578,16 @@
         <v>47</v>
       </c>
       <c r="C113" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E113" t="s">
         <v>1605</v>
       </c>
-      <c r="D113" t="s">
-        <v>1605</v>
-      </c>
-      <c r="E113" t="s">
+      <c r="F113" t="s">
         <v>1606</v>
-      </c>
-      <c r="F113" t="s">
-        <v>1607</v>
       </c>
       <c r="G113" t="s">
         <v>0</v>
@@ -17679,7 +17680,7 @@
         <v>0</v>
       </c>
       <c r="AK113" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="AL113" t="s">
         <v>53</v>
@@ -17693,16 +17694,16 @@
         <v>54</v>
       </c>
       <c r="C114" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E114" t="s">
         <v>1605</v>
       </c>
-      <c r="D114" t="s">
-        <v>1605</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>1606</v>
-      </c>
-      <c r="F114" t="s">
-        <v>1607</v>
       </c>
       <c r="G114" t="s">
         <v>156</v>
@@ -17711,7 +17712,7 @@
         <v>93</v>
       </c>
       <c r="I114" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="J114" t="s">
         <v>58</v>
@@ -17809,16 +17810,16 @@
         <v>47</v>
       </c>
       <c r="C115" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D115" t="s">
+        <v>1609</v>
+      </c>
+      <c r="E115" t="s">
         <v>1610</v>
       </c>
-      <c r="D115" t="s">
-        <v>1610</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="F115" t="s">
         <v>1611</v>
-      </c>
-      <c r="F115" t="s">
-        <v>1612</v>
       </c>
       <c r="G115" t="s">
         <v>0</v>
@@ -17911,7 +17912,7 @@
         <v>0</v>
       </c>
       <c r="AK115" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="AL115" t="s">
         <v>53</v>
@@ -17925,25 +17926,25 @@
         <v>54</v>
       </c>
       <c r="C116" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1609</v>
+      </c>
+      <c r="E116" t="s">
         <v>1610</v>
       </c>
-      <c r="D116" t="s">
-        <v>1610</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="F116" t="s">
         <v>1611</v>
       </c>
-      <c r="F116" t="s">
-        <v>1612</v>
-      </c>
       <c r="G116" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="H116" t="s">
         <v>179</v>
       </c>
       <c r="I116" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="J116" t="s">
         <v>58</v>
@@ -18041,16 +18042,16 @@
         <v>47</v>
       </c>
       <c r="C117" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E117" t="s">
         <v>1616</v>
       </c>
-      <c r="D117" t="s">
-        <v>1616</v>
-      </c>
-      <c r="E117" t="s">
+      <c r="F117" t="s">
         <v>1617</v>
-      </c>
-      <c r="F117" t="s">
-        <v>1618</v>
       </c>
       <c r="G117" t="s">
         <v>0</v>
@@ -18143,7 +18144,7 @@
         <v>0</v>
       </c>
       <c r="AK117" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="AL117" t="s">
         <v>53</v>
@@ -18157,16 +18158,16 @@
         <v>54</v>
       </c>
       <c r="C118" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D118" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E118" t="s">
         <v>1616</v>
       </c>
-      <c r="D118" t="s">
-        <v>1616</v>
-      </c>
-      <c r="E118" t="s">
+      <c r="F118" t="s">
         <v>1617</v>
-      </c>
-      <c r="F118" t="s">
-        <v>1618</v>
       </c>
       <c r="G118" t="s">
         <v>499</v>
@@ -18175,7 +18176,7 @@
         <v>150</v>
       </c>
       <c r="I118" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="J118" t="s">
         <v>58</v>
@@ -18273,16 +18274,16 @@
         <v>47</v>
       </c>
       <c r="C119" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1620</v>
+      </c>
+      <c r="E119" t="s">
         <v>1621</v>
       </c>
-      <c r="D119" t="s">
-        <v>1621</v>
-      </c>
-      <c r="E119" t="s">
+      <c r="F119" t="s">
         <v>1622</v>
-      </c>
-      <c r="F119" t="s">
-        <v>1623</v>
       </c>
       <c r="G119" t="s">
         <v>0</v>
@@ -18375,7 +18376,7 @@
         <v>0</v>
       </c>
       <c r="AK119" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="AL119" t="s">
         <v>53</v>
@@ -18389,25 +18390,25 @@
         <v>54</v>
       </c>
       <c r="C120" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1620</v>
+      </c>
+      <c r="E120" t="s">
         <v>1621</v>
       </c>
-      <c r="D120" t="s">
-        <v>1621</v>
-      </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>1622</v>
       </c>
-      <c r="F120" t="s">
-        <v>1623</v>
-      </c>
       <c r="G120" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="H120" t="s">
         <v>220</v>
       </c>
       <c r="I120" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="J120" t="s">
         <v>58</v>
@@ -18505,16 +18506,16 @@
         <v>47</v>
       </c>
       <c r="C121" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1626</v>
+      </c>
+      <c r="E121" t="s">
         <v>1627</v>
       </c>
-      <c r="D121" t="s">
-        <v>1627</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="F121" t="s">
         <v>1628</v>
-      </c>
-      <c r="F121" t="s">
-        <v>1629</v>
       </c>
       <c r="G121" t="s">
         <v>0</v>
@@ -18607,7 +18608,7 @@
         <v>0</v>
       </c>
       <c r="AK121" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="AL121" t="s">
         <v>53</v>
@@ -18621,16 +18622,16 @@
         <v>54</v>
       </c>
       <c r="C122" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1626</v>
+      </c>
+      <c r="E122" t="s">
         <v>1627</v>
       </c>
-      <c r="D122" t="s">
-        <v>1627</v>
-      </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>1628</v>
-      </c>
-      <c r="F122" t="s">
-        <v>1629</v>
       </c>
       <c r="G122" t="s">
         <v>150</v>
@@ -18639,7 +18640,7 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="J122" t="s">
         <v>58</v>
@@ -24811,7 +24812,7 @@
         <v>0</v>
       </c>
       <c r="Q175" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R175">
         <v>406115946334</v>
@@ -25275,7 +25276,7 @@
         <v>0</v>
       </c>
       <c r="Q179" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R179">
         <v>406160827276</v>
@@ -25507,7 +25508,7 @@
         <v>0</v>
       </c>
       <c r="Q181" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R181">
         <v>406155629578</v>
@@ -25739,7 +25740,7 @@
         <v>0</v>
       </c>
       <c r="Q183" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R183">
         <v>406142479393</v>
@@ -26203,7 +26204,7 @@
         <v>0</v>
       </c>
       <c r="Q187" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R187">
         <v>406126420661</v>
@@ -26435,7 +26436,7 @@
         <v>0</v>
       </c>
       <c r="Q189" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R189">
         <v>406136806041</v>
@@ -27131,7 +27132,7 @@
         <v>0</v>
       </c>
       <c r="Q195" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R195">
         <v>406142372232</v>
@@ -28059,7 +28060,7 @@
         <v>0</v>
       </c>
       <c r="Q203" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R203">
         <v>406142024065</v>
@@ -28291,7 +28292,7 @@
         <v>0</v>
       </c>
       <c r="Q205" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R205">
         <v>406115946334</v>
@@ -28523,7 +28524,7 @@
         <v>0</v>
       </c>
       <c r="Q207" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R207">
         <v>406160827276</v>
@@ -28987,7 +28988,7 @@
         <v>0</v>
       </c>
       <c r="Q211" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R211">
         <v>406115946334</v>
@@ -29335,7 +29336,7 @@
         <v>0</v>
       </c>
       <c r="Q214" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="R214">
         <v>406115946334</v>
@@ -29451,7 +29452,7 @@
         <v>0</v>
       </c>
       <c r="Q215" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R215">
         <v>406160827276</v>
@@ -29915,7 +29916,7 @@
         <v>0</v>
       </c>
       <c r="Q219" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R219">
         <v>406160827276</v>
@@ -30495,7 +30496,7 @@
         <v>0</v>
       </c>
       <c r="Q224" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R224">
         <v>406160827276</v>
@@ -32467,7 +32468,7 @@
         <v>0</v>
       </c>
       <c r="Q241" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="R241">
         <v>406142372232</v>
@@ -35251,7 +35252,7 @@
         <v>0</v>
       </c>
       <c r="Q265" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="R265">
         <v>406115946334</v>
@@ -47431,7 +47432,7 @@
         <v>0</v>
       </c>
       <c r="Q370" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="R370">
         <v>406142372232</v>
@@ -63787,7 +63788,7 @@
         <v>0</v>
       </c>
       <c r="Q511" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="R511">
         <v>406123550928</v>

</xml_diff>